<commit_message>
Minor updates, add imgs, update readme.md, add requirements.txt
</commit_message>
<xml_diff>
--- a/data/order.xlsx
+++ b/data/order.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\excel_console_app\excel_console_app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D71B37-0BBD-4E72-AAC4-26A3F1910505}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C32FBCD-D6E1-4A3B-8E1A-B9C9669F2380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TDSheet" sheetId="1" r:id="rId1"/>
@@ -828,7 +828,7 @@
   <dimension ref="A1:G52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>

</xml_diff>